<commit_message>
added esr and pl error colour code
</commit_message>
<xml_diff>
--- a/excel/Products/stockData.xlsx
+++ b/excel/Products/stockData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="67">
   <si>
     <t>Symbol</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Internal Closing Price</t>
+  </si>
+  <si>
+    <t>today</t>
   </si>
 </sst>
 </file>
@@ -1123,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1143,7 +1146,7 @@
     <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1171,8 +1174,11 @@
       <c r="I1" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1198,16 +1204,19 @@
         <v>29</v>
       </c>
       <c r="I2" s="4">
-        <v>82.1</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="J2" s="4">
-        <v>82.1</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="K2" s="1">
         <v>82.45</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L2" s="4">
+        <v>82.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1233,16 +1242,19 @@
         <v>30</v>
       </c>
       <c r="I3" s="1">
-        <v>14.9</v>
+        <v>14.88</v>
       </c>
       <c r="J3" s="1">
-        <v>14.9</v>
+        <v>14.88</v>
       </c>
       <c r="K3" s="1">
         <v>15.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L3" s="1">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1268,16 +1280,19 @@
         <v>31</v>
       </c>
       <c r="I4" s="1">
-        <v>65.55</v>
+        <v>65.5</v>
       </c>
       <c r="J4" s="1">
-        <v>65.55</v>
+        <v>65.5</v>
       </c>
       <c r="K4" s="1">
         <v>66.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L4" s="1">
+        <v>65.55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1303,16 +1318,19 @@
         <v>32</v>
       </c>
       <c r="I5" s="1">
-        <v>75.150000000000006</v>
+        <v>75.349999999999994</v>
       </c>
       <c r="J5" s="1">
-        <v>75.150000000000006</v>
+        <v>75.349999999999994</v>
       </c>
       <c r="K5" s="1">
         <v>63.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L5" s="1">
+        <v>75.150000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -1338,16 +1356,19 @@
         <v>32</v>
       </c>
       <c r="I6" s="1">
-        <v>75.150000000000006</v>
+        <v>75.349999999999994</v>
       </c>
       <c r="J6" s="1">
-        <v>75.150000000000006</v>
+        <v>75.349999999999994</v>
       </c>
       <c r="K6" s="1">
         <v>63.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L6" s="1">
+        <v>75.150000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1373,16 +1394,19 @@
         <v>33</v>
       </c>
       <c r="I7" s="1">
-        <v>68.5</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="J7" s="1">
-        <v>68.5</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="K7" s="1">
         <v>68.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L7" s="1">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1408,16 +1432,19 @@
         <v>34</v>
       </c>
       <c r="I8" s="1">
-        <v>165.2</v>
+        <v>165</v>
       </c>
       <c r="J8" s="1">
-        <v>165.2</v>
+        <v>165</v>
       </c>
       <c r="K8" s="1">
         <v>157.69999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L8" s="1">
+        <v>165.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1443,16 +1470,19 @@
         <v>35</v>
       </c>
       <c r="I9" s="1">
-        <v>44.65</v>
+        <v>50</v>
       </c>
       <c r="J9" s="1">
-        <v>44.65</v>
+        <v>46.1</v>
       </c>
       <c r="K9" s="1">
         <v>49.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L9" s="1">
+        <v>44.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
@@ -1478,16 +1508,19 @@
         <v>36</v>
       </c>
       <c r="I10" s="1">
-        <v>119.3</v>
+        <v>119</v>
       </c>
       <c r="J10" s="1">
-        <v>119.3</v>
+        <v>119</v>
       </c>
       <c r="K10" s="1">
         <v>117.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L10" s="1">
+        <v>119.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1513,16 +1546,19 @@
         <v>36</v>
       </c>
       <c r="I11" s="1">
-        <v>119.3</v>
+        <v>119</v>
       </c>
       <c r="J11" s="1">
-        <v>119.3</v>
+        <v>119</v>
       </c>
       <c r="K11" s="1">
         <v>117.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L11" s="1">
+        <v>119.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1548,16 +1584,19 @@
         <v>36</v>
       </c>
       <c r="I12" s="1">
-        <v>119.3</v>
+        <v>119</v>
       </c>
       <c r="J12" s="1">
-        <v>119.3</v>
+        <v>119</v>
       </c>
       <c r="K12" s="1">
         <v>117.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L12" s="1">
+        <v>119.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1583,16 +1622,19 @@
         <v>37</v>
       </c>
       <c r="I13" s="1">
-        <v>10.28</v>
+        <v>10.24</v>
       </c>
       <c r="J13" s="1">
-        <v>10.28</v>
+        <v>10.24</v>
       </c>
       <c r="K13" s="1">
         <v>9.75</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L13" s="1">
+        <v>10.28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1626,8 +1668,11 @@
       <c r="K14" s="1">
         <v>78.099999999999994</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L14" s="1">
+        <v>76.849999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1653,16 +1698,19 @@
         <v>39</v>
       </c>
       <c r="I15" s="1">
-        <v>33.700000000000003</v>
+        <v>33.85</v>
       </c>
       <c r="J15" s="1">
-        <v>33.700000000000003</v>
+        <v>33.85</v>
       </c>
       <c r="K15" s="1">
         <v>32.15</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L15" s="1">
+        <v>33.700000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
@@ -1688,16 +1736,19 @@
         <v>39</v>
       </c>
       <c r="I16" s="1">
-        <v>33.700000000000003</v>
+        <v>33.85</v>
       </c>
       <c r="J16" s="1">
-        <v>33.700000000000003</v>
+        <v>33.85</v>
       </c>
       <c r="K16" s="1">
         <v>32.15</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L16" s="1">
+        <v>33.700000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1723,16 +1774,19 @@
         <v>40</v>
       </c>
       <c r="I17" s="1">
-        <v>44.65</v>
+        <v>44.55</v>
       </c>
       <c r="J17" s="1">
-        <v>44.65</v>
+        <v>46.1</v>
       </c>
       <c r="K17" s="1">
         <v>44.45</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L17" s="1">
+        <v>44.65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1758,16 +1812,19 @@
         <v>41</v>
       </c>
       <c r="I18" s="1">
-        <v>13.04</v>
+        <v>12.96</v>
       </c>
       <c r="J18" s="1">
-        <v>13.04</v>
+        <v>12.96</v>
       </c>
       <c r="K18" s="1">
         <v>13.48</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L18" s="1">
+        <v>13.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1793,16 +1850,19 @@
         <v>42</v>
       </c>
       <c r="I19" s="1">
-        <v>19.899999999999999</v>
+        <v>19.62</v>
       </c>
       <c r="J19" s="1">
-        <v>19.899999999999999</v>
+        <v>19.62</v>
       </c>
       <c r="K19" s="1">
         <v>20.65</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L19" s="1">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1828,16 +1888,19 @@
         <v>43</v>
       </c>
       <c r="I20" s="1">
-        <v>7.44</v>
+        <v>7.39</v>
       </c>
       <c r="J20" s="1">
-        <v>7.44</v>
+        <v>7.39</v>
       </c>
       <c r="K20" s="1">
         <v>7.95</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L20" s="1">
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
@@ -1863,16 +1926,19 @@
         <v>44</v>
       </c>
       <c r="I21" s="1">
-        <v>22.4</v>
+        <v>23.55</v>
       </c>
       <c r="J21" s="1">
-        <v>22.4</v>
+        <v>23.55</v>
       </c>
       <c r="K21" s="1">
         <v>22.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L21" s="1">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1898,16 +1964,19 @@
         <v>45</v>
       </c>
       <c r="I22" s="1">
-        <v>5.37</v>
+        <v>5.31</v>
       </c>
       <c r="J22" s="1">
-        <v>5.37</v>
+        <v>5.31</v>
       </c>
       <c r="K22" s="1">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L22" s="1">
+        <v>5.37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1933,16 +2002,19 @@
         <v>46</v>
       </c>
       <c r="I23" s="5">
-        <v>18.559999999999999</v>
+        <v>18.7</v>
       </c>
       <c r="J23" s="5">
-        <v>18.559999999999999</v>
+        <v>18.7</v>
       </c>
       <c r="K23" s="1">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L23" s="5">
+        <v>18.559999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -1967,17 +2039,20 @@
       <c r="H24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I24" s="1">
-        <v>18.559999999999999</v>
-      </c>
-      <c r="J24" s="1">
-        <v>18.559999999999999</v>
+      <c r="I24" s="5">
+        <v>18.7</v>
+      </c>
+      <c r="J24" s="5">
+        <v>18.7</v>
       </c>
       <c r="K24" s="1">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L24" s="1">
+        <v>18.559999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -2003,16 +2078,19 @@
         <v>47</v>
       </c>
       <c r="I25" s="1">
-        <v>11.78</v>
+        <v>11.72</v>
       </c>
       <c r="J25" s="1">
-        <v>11.78</v>
+        <v>11.72</v>
       </c>
       <c r="K25" s="1">
         <v>11.02</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L25" s="1">
+        <v>11.78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -2038,16 +2116,19 @@
         <v>48</v>
       </c>
       <c r="I26" s="1">
-        <v>12.72</v>
+        <v>12.58</v>
       </c>
       <c r="J26" s="1">
-        <v>12.72</v>
+        <v>12.58</v>
       </c>
       <c r="K26" s="1">
         <v>11.16</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L26" s="1">
+        <v>12.72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2073,16 +2154,19 @@
         <v>49</v>
       </c>
       <c r="I27" s="1">
-        <v>209.8</v>
+        <v>211.8</v>
       </c>
       <c r="J27" s="1">
-        <v>209.8</v>
+        <v>211.8</v>
       </c>
       <c r="K27" s="1">
         <v>195.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L27" s="1">
+        <v>209.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -2108,16 +2192,19 @@
         <v>50</v>
       </c>
       <c r="I28" s="1">
-        <v>284.8</v>
+        <v>285</v>
       </c>
       <c r="J28" s="1">
-        <v>284.8</v>
+        <v>285</v>
       </c>
       <c r="K28" s="1">
         <v>226.4</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L28" s="1">
+        <v>284.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
@@ -2143,16 +2230,19 @@
         <v>50</v>
       </c>
       <c r="I29" s="1">
-        <v>284.8</v>
+        <v>285</v>
       </c>
       <c r="J29" s="1">
-        <v>284.8</v>
+        <v>285</v>
       </c>
       <c r="K29" s="1">
         <v>226.4</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="L29" s="1">
+        <v>284.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <autoFilter ref="A1:I29"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>